<commit_message>
manda dato de guardado
Manda el dato al esp32 par aque el neoxpixel se encienda
</commit_message>
<xml_diff>
--- a/Pinout PROYECTO 3.xlsx
+++ b/Pinout PROYECTO 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\SEMESTRE DE LA U\6TO SEMESTRE\DIGITAL 2\PROYECTO 3\PROYECTO_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E4D58B-873A-447D-91FD-D1AA1799B058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F0F092-C700-4C4D-B437-802FF2C4F8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33FA0D3F-264E-4F2D-8D17-345DFAF046CD}"/>
   </bookViews>
@@ -294,12 +294,6 @@
     <t>Rx2</t>
   </si>
   <si>
-    <t>RX3</t>
-  </si>
-  <si>
-    <t>TX3</t>
-  </si>
-  <si>
     <t>LCD_RST</t>
   </si>
   <si>
@@ -424,6 +418,12 @@
   </si>
   <si>
     <t>RX2</t>
+  </si>
+  <si>
+    <t>RX4</t>
+  </si>
+  <si>
+    <t>TX4</t>
   </si>
 </sst>
 </file>
@@ -575,11 +575,11 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65D1A52-722E-4D88-830B-F2F29FFF5A54}">
   <dimension ref="A3:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1243,10 +1243,10 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1260,15 +1260,15 @@
         <v>19</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="2" t="s">
@@ -1282,10 +1282,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="2" t="s">
@@ -1299,10 +1299,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="2" t="s">
@@ -1314,12 +1314,12 @@
         <v>22</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>87</v>
@@ -1377,7 +1377,7 @@
         <v>28</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1393,7 +1393,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1429,8 +1429,8 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="E15" s="28" t="s">
-        <v>129</v>
+      <c r="E15" s="27" t="s">
+        <v>127</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
@@ -1443,10 +1443,10 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40" s="16" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>83</v>
@@ -1682,7 +1682,7 @@
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C46" s="27"/>
+      <c r="C46" s="26"/>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
       <c r="F46" s="10" t="s">
@@ -1702,13 +1702,13 @@
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B47" s="16" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>84</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="10" t="s">
@@ -1725,21 +1725,21 @@
       </c>
       <c r="N47" s="11"/>
       <c r="O47" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B48" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>35</v>
@@ -1754,22 +1754,22 @@
         <v>55</v>
       </c>
       <c r="N48" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O48" s="11"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B49" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>37</v>
@@ -1783,18 +1783,21 @@
       <c r="M49" s="10" t="s">
         <v>56</v>
       </c>
+      <c r="N49" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="O49" s="11"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B50" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>39</v>
@@ -1808,18 +1811,21 @@
       <c r="M50" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="N50" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="O50" s="11"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B51" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>41</v>
@@ -1833,25 +1839,22 @@
       <c r="M51" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="N51" s="14" t="s">
-        <v>86</v>
-      </c>
       <c r="O51" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B52" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -1865,22 +1868,19 @@
       <c r="M52" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="N52" s="14" t="s">
-        <v>85</v>
-      </c>
       <c r="O52" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B53" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="10" t="s">
@@ -1897,15 +1897,15 @@
       </c>
       <c r="N53" s="11"/>
       <c r="O53" s="25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B54" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
@@ -1923,15 +1923,15 @@
       </c>
       <c r="N54" s="11"/>
       <c r="O54" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B55" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
@@ -1949,15 +1949,15 @@
       </c>
       <c r="N55" s="11"/>
       <c r="O55" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B56" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -1966,10 +1966,10 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B57" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
@@ -1978,10 +1978,10 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B58" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -1990,10 +1990,10 @@
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B59" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -2002,42 +2002,42 @@
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B60" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B63" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B64" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nombre de la función
Se cambio el nombre de la función por el verdadero nombre
</commit_message>
<xml_diff>
--- a/Pinout PROYECTO 3.xlsx
+++ b/Pinout PROYECTO 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\SEMESTRE DE LA U\6TO SEMESTRE\DIGITAL 2\PROYECTO 3\PROYECTO_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F0F092-C700-4C4D-B437-802FF2C4F8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B0C877-1ED5-4372-93DE-9785F41305A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33FA0D3F-264E-4F2D-8D17-345DFAF046CD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
   <si>
     <t>Entradas</t>
   </si>
@@ -268,12 +268,6 @@
   </si>
   <si>
     <t>PF_0</t>
-  </si>
-  <si>
-    <t>GPIO14</t>
-  </si>
-  <si>
-    <t>ECHO</t>
   </si>
   <si>
     <t>PC_4</t>
@@ -1221,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65D1A52-722E-4D88-830B-F2F29FFF5A54}">
   <dimension ref="A3:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,15 +1254,15 @@
         <v>19</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="2" t="s">
@@ -1282,10 +1276,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>126</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="2" t="s">
@@ -1299,10 +1293,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="2" t="s">
@@ -1314,15 +1308,15 @@
         <v>22</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="2" t="s">
@@ -1377,7 +1371,7 @@
         <v>28</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1393,7 +1387,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1430,7 +1424,7 @@
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="E15" s="27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
@@ -1461,11 +1455,11 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
-      <c r="B17" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>81</v>
+      <c r="B17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>3</v>
@@ -1478,12 +1472,6 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
-      <c r="B18" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1607,10 +1595,10 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
@@ -1702,13 +1690,13 @@
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B47" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="10" t="s">
@@ -1725,21 +1713,21 @@
       </c>
       <c r="N47" s="11"/>
       <c r="O47" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B48" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>35</v>
@@ -1754,22 +1742,22 @@
         <v>55</v>
       </c>
       <c r="N48" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O48" s="11"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B49" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>37</v>
@@ -1784,20 +1772,20 @@
         <v>56</v>
       </c>
       <c r="N49" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O49" s="11"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B50" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>39</v>
@@ -1812,20 +1800,20 @@
         <v>59</v>
       </c>
       <c r="N50" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O50" s="11"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B51" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>41</v>
@@ -1840,21 +1828,21 @@
         <v>60</v>
       </c>
       <c r="O51" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B52" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>44</v>
@@ -1869,18 +1857,18 @@
         <v>63</v>
       </c>
       <c r="O52" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B53" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="10" t="s">
@@ -1897,15 +1885,15 @@
       </c>
       <c r="N53" s="11"/>
       <c r="O53" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B54" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
@@ -1923,15 +1911,15 @@
       </c>
       <c r="N54" s="11"/>
       <c r="O54" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B55" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
@@ -1949,15 +1937,15 @@
       </c>
       <c r="N55" s="11"/>
       <c r="O55" s="25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B56" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -1966,10 +1954,10 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B57" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
@@ -1978,10 +1966,10 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B58" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -1990,10 +1978,10 @@
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B59" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -2002,42 +1990,42 @@
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B60" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B63" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B64" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>